<commit_message>
Modify some changes in bug metrics and testcases
Co-Authored-By: j1em1n <j1em1n@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HuiSin\Documents\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA981EB-A51F-494F-8285-7353711C7E3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68078EE-0F92-4C3E-9B60-ED88427841F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -403,13 +403,13 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,7 +922,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -995,7 +995,7 @@
       <c r="F3" s="20">
         <v>5</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="28">
         <v>26</v>
       </c>
       <c r="H3" s="24" t="str">
@@ -1022,7 +1022,7 @@
       <c r="F4" s="20">
         <v>1</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
       <c r="F5" s="20">
         <v>5</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
@@ -1065,7 +1065,7 @@
       <c r="F6" s="20">
         <v>5</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
@@ -1086,7 +1086,7 @@
       <c r="F7" s="20">
         <v>10</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
@@ -6338,16 +6338,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
added padZeroTime() function to common.php
Co-Authored-By: huisinnnn <huisinnnn@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CF3458-319A-4975-AA3E-C4CED79BA5DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCB524E-25F6-4C70-A280-90D7C7AFA4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
   <si>
     <t>Bug Log</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Too few arguments in 'validateDate()'</t>
+  </si>
+  <si>
+    <t>Column not found: Unknown column 'round_number' in line 32 of RoundDAO.php</t>
+  </si>
+  <si>
+    <t>Incorrect row numbers shown in bootstrap errors</t>
+  </si>
+  <si>
+    <t>Issue with the validateDate() function in common.php, causing all course rows to be ignored</t>
   </si>
 </sst>
 </file>
@@ -936,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1194,23 +1203,39 @@
       <c r="B12" s="25">
         <v>2</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20" t="str">
+      <c r="C12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="20">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>11</v>
       </c>
       <c r="B13" s="25">
         <v>2</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20" t="str">
+      <c r="C13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="20">
         <f t="shared" si="1"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
@@ -1220,10 +1245,18 @@
       <c r="B14" s="25">
         <v>2</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20" t="str">
+      <c r="C14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="20">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
forgot to commit test cases and bm (bootstrap)
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffi\Documents\GitHub\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCB524E-25F6-4C70-A280-90D7C7AFA4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D919E5A0-BA67-47B9-9FAE-CAA545FF99EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="19536" windowHeight="10473" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
   <si>
     <t>Bug Log</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Issue with the validateDate() function in common.php, causing all course rows to be ignored</t>
+  </si>
+  <si>
+    <t>A non well formed numeric value encountered (used wrong symbol to concatenate strings in PHP)</t>
   </si>
 </sst>
 </file>
@@ -946,7 +949,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1259,15 +1262,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="29.2" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>13</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20" t="str">
+      <c r="B15" s="25">
+        <v>2</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="20">
         <f t="shared" si="1"/>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
debug drop bid functionality and added printSuccess function in common.php and testcases for drop bid
Co-Authored-By: huisinnnn <huisinnnn@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mygit\project-g1t8\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A96F233-3DEC-42C8-B400-D2FCFA715994}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED61D942-6C84-4581-B179-D51A517B0323}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,13 +557,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -575,42 +568,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,6 +584,49 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,16 +1156,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -1194,408 +1194,408 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="27">
         <v>5</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="36">
         <v>26</v>
       </c>
-      <c r="H3" s="37" t="str">
+      <c r="H3" s="40" t="str">
         <f xml:space="preserve"> IF(G3&lt;10,Instructions!B7,Instructions!B8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="27">
         <v>2</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="27">
         <v>1</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="38"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="27">
         <v>3</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="27">
         <v>1</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="27">
         <v>5</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="38"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="27">
         <v>4</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="27">
         <v>1</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="27">
         <v>5</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="38"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="27">
         <v>5</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="27">
         <v>1</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="27">
         <v>10</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="39"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="30">
+      <c r="A8" s="27">
         <v>6</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>2.1</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="27">
         <v>5</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="36">
         <v>15</v>
       </c>
-      <c r="H8" s="40" t="str">
+      <c r="H8" s="38" t="str">
         <f xml:space="preserve"> IF(G6&lt;10,Instructions!B7,Instructions!B8)</f>
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="30">
+      <c r="A9" s="27">
         <v>7</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="29">
         <v>2.1</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="27">
         <v>5</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="41"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="30">
+      <c r="A10" s="27">
         <v>8</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="29">
         <v>2.1</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="27">
         <v>5</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="42"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="27">
         <v>9</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="27">
         <v>10</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="36">
         <v>20</v>
       </c>
-      <c r="H11" s="37" t="str">
+      <c r="H11" s="40" t="str">
         <f xml:space="preserve"> IF(G11&lt;10,Instructions!B7,Instructions!B8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="27">
         <v>10</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="27">
         <v>10</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="39"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="27">
         <v>11</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="27">
         <v>10</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="36">
         <v>20</v>
       </c>
-      <c r="H13" s="37" t="str">
+      <c r="H13" s="40" t="str">
         <f xml:space="preserve"> IF(G13&lt;10,Instructions!B7,Instructions!B8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30">
+      <c r="A14" s="27">
         <v>12</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="27">
         <v>10</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="39"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30">
+      <c r="A15" s="27">
         <v>13</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="27">
         <v>10</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="36">
         <v>15</v>
       </c>
-      <c r="H15" s="43" t="str">
+      <c r="H15" s="42" t="str">
         <f xml:space="preserve"> IF(G15&lt;10,Instructions!B7,Instructions!B8)</f>
         <v>Stop current development and resolve the bug immediately. Project Manager reschedules the project.</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46">
+      <c r="A16" s="31">
         <v>14</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="27">
         <v>5</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="44"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47">
+      <c r="A17" s="32">
         <v>15</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="27">
         <v>1</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="45"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="44"/>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47">
+      <c r="A18" s="32">
         <v>16</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="27">
         <v>5</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="36">
         <v>6</v>
       </c>
-      <c r="H18" s="40" t="str">
+      <c r="H18" s="38" t="str">
         <f xml:space="preserve"> IF(G18&lt;10,Instructions!B7,Instructions!B8)</f>
         <v>Use the planned debugging time in the iteration.</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49">
+      <c r="A19" s="34">
         <v>17</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B19" s="35">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="27">
         <v>1</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="42"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="39"/>
     </row>
     <row r="20" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
@@ -1604,7 +1604,7 @@
       <c r="B20" s="25"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20" t="str">
-        <f t="shared" ref="F18:F181" si="0">IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
+        <f t="shared" ref="F20:F181" si="0">IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v/>
       </c>
     </row>
@@ -6676,6 +6676,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="G11:G12"/>
@@ -6684,11 +6689,6 @@
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="G3:G7"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2 H20:H1048576">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Stop current Development">
@@ -6727,16 +6727,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">

</xml_diff>